<commit_message>
Change the policy of output YAML file.
Each sheet included in excel file will be writen by each sheet.
</commit_message>
<xml_diff>
--- a/sample_data/sample_auth.xlsx
+++ b/sample_data/sample_auth.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="0" windowWidth="27860" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="0" windowWidth="27860" windowHeight="16080" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="auth" sheetId="1" r:id="rId1"/>
+    <sheet name="Note" sheetId="3" r:id="rId1"/>
+    <sheet name="plain-text" sheetId="1" r:id="rId2"/>
+    <sheet name="public-key" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>cisco</t>
     <phoneticPr fontId="1"/>
@@ -33,42 +35,69 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Update Date:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>defalt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>renat</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>password!</t>
+  </si>
+  <si>
+    <t>Update Date: 1984/09/01 by yuji</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>$USER</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>$HOME/.ssh/robot_id_rsa</t>
+  </si>
+  <si>
+    <t>key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Title: B1 DC base setting</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Comment: Base setting</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>Title:</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Update Date:</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>defalt</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>renat</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>user</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>password!</t>
   </si>
   <si>
     <t>Comment:</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>* This sheet is free format and will not be transformed to YAML file.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,6 +140,29 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -135,7 +187,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -145,25 +197,51 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="19">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -492,7 +570,439 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="49.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="18" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -506,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -518,7 +1028,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -530,7 +1040,7 @@
     </row>
     <row r="3" spans="1:8" ht="18" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -545,43 +1055,21 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete description from each excel sheet
</commit_message>
<xml_diff>
--- a/sample_data/sample_auth.xlsx
+++ b/sample_data/sample_auth.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="0" windowWidth="27860" windowHeight="16080" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="4220" yWindow="40" windowWidth="27860" windowHeight="16080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Note" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>cisco</t>
     <phoneticPr fontId="1"/>
@@ -35,10 +35,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Update Date:</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>defalt</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -73,31 +69,22 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Title: B1 DC base setting</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Comment: Base setting</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Title:</t>
-  </si>
-  <si>
-    <t>Update Date:</t>
-  </si>
-  <si>
-    <t>Comment:</t>
-  </si>
-  <si>
     <t>* This sheet is free format and will not be transformed to YAML file.</t>
+  </si>
+  <si>
+    <t>Title: [TEST 3-1-1] Single chassis topology</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Comment: Single chassis topology at B1 DC</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,15 +124,6 @@
       <color theme="11"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -208,7 +186,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -217,10 +195,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -572,316 +546,292 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="A27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -896,11 +846,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
@@ -908,84 +856,48 @@
     <col min="6" max="6" width="49.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1002,10 +914,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1014,62 +926,26 @@
     <col min="6" max="6" width="49.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C2" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>